<commit_message>
Implement product deletion functionality and UI updates
- Modified `BancoDados.xlsx` (binary changes).
- Adjusted `TabIndex` properties and corrected labels in `AddProductForm.Designer.cs`.
- Added `DeleteProduct` method in `AddProductForm.cs` for product deletion.
- Enhanced `DetailForm` layout with a delete button and updated text box order.
- Implemented deletion functionality in `DetailForm.cs` with user confirmation.
- Added `Delete` method in `ExcelProductRepository.cs` for Excel record removal.
- Updated `IProductRepository.cs` to include the `Delete` method.
- Enhanced `ProductService.cs` with a method for deleting products.
- Cleaned up `Program.cs` by removing commented-out code for clarity.
</commit_message>
<xml_diff>
--- a/BancoDados.xlsx
+++ b/BancoDados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio7\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio7\source\repos\HistoricoDefeitosProduto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A08F233-90D0-4B4C-88B8-30802B87F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1391E9-C326-43ED-A07A-E42E420F8126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB21EB93-9644-4518-B985-D358FBFF11AD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Funcionario</t>
   </si>
@@ -71,126 +71,90 @@
     <t>DesDataHoracricao</t>
   </si>
   <si>
-    <t>Caio Cesar</t>
+    <t>Caio Gonzaga</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>FE04</t>
-  </si>
-  <si>
-    <t>FE Fresh</t>
+    <t>FE01</t>
+  </si>
+  <si>
+    <t>FE FRESH</t>
   </si>
   <si>
     <t>ZF5254T7ZL</t>
   </si>
   <si>
-    <t>Lamu</t>
-  </si>
-  <si>
-    <t>Cold soldering</t>
+    <t>LAMU</t>
+  </si>
+  <si>
+    <t>Displaced weld deposition</t>
   </si>
   <si>
     <t>Solder</t>
   </si>
   <si>
-    <t>Bad reflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foi feito tal coisa.
-Calibração de tal coisa.</t>
-  </si>
-  <si>
-    <t>3/17/2025 12:33 AM</t>
+    <t>Shifted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste.
+Teste.</t>
+  </si>
+  <si>
+    <t>3/17/2025 3:50 PM</t>
   </si>
   <si>
     <t>Bruno Auzier</t>
   </si>
   <si>
+    <t>FE05</t>
+  </si>
+  <si>
+    <t>Lack of PM, obstructed, damaged, worn, life time, etc.</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Nozzle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste.
+Tese.</t>
+  </si>
+  <si>
+    <t>3/17/2025 3:51 PM</t>
+  </si>
+  <si>
+    <t>Maycon Nascimento</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>FE05</t>
-  </si>
-  <si>
-    <t>BE Fresh</t>
-  </si>
-  <si>
-    <t>Problems with humidity, temperature, dust, etc.</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Enviroment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feito tal.
-Calibração de tal.
-Mais tal.
-</t>
-  </si>
-  <si>
-    <t>3/17/2025 12:35 AM</t>
-  </si>
-  <si>
-    <t>Maycon Nascimento</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>BE07</t>
+  </si>
+  <si>
+    <t>BE FRESH</t>
   </si>
   <si>
     <t>ZF5254T7XJ</t>
   </si>
   <si>
-    <t>Manila</t>
-  </si>
-  <si>
-    <t>Lack of PM, damaged, life time, CM, calibration, transport error etc</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Conveyor Mounter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feito tal coisa;
-Mais isso.</t>
-  </si>
-  <si>
-    <t>3/17/2025 12:36 AM</t>
-  </si>
-  <si>
-    <t>Victor Barbosa</t>
-  </si>
-  <si>
-    <t>FE08</t>
-  </si>
-  <si>
-    <t>Bone</t>
-  </si>
-  <si>
-    <t>Lack of trained people at the post</t>
-  </si>
-  <si>
-    <t>Absenteeism</t>
-  </si>
-  <si>
-    <t>Feito tal coisa.</t>
-  </si>
-  <si>
-    <t>3/17/2025 12:44 AM</t>
-  </si>
-  <si>
-    <t>Caio Gonzaga</t>
-  </si>
-  <si>
-    <t>Teste</t>
-  </si>
-  <si>
-    <t>3/17/2025 1:07 AM</t>
+    <t>MANILA</t>
+  </si>
+  <si>
+    <t>Engineering activities (Process engineering, maintenance, testing, product, etc.)</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Beta process</t>
+  </si>
+  <si>
+    <t>3/17/2025 3:53 PM</t>
   </si>
 </sst>
 </file>
@@ -588,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F50CB-CCF4-4A02-8BB3-6545B4B7DBF8}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,13 +648,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>15</v>
@@ -699,33 +663,33 @@
         <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>33</v>
@@ -743,84 +707,14 @@
         <v>37</v>
       </c>
       <c r="J4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Update in database data and path
</commit_message>
<xml_diff>
--- a/BancoDados.xlsx
+++ b/BancoDados.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio7\source\repos\HistoricoDefeitosProduto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnscgonz\source\repos\caiogonz\HistoricoDefeitosProduto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1391E9-C326-43ED-A07A-E42E420F8126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB21EB93-9644-4518-B985-D358FBFF11AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Defeitos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Funcionario</t>
   </si>
@@ -68,7 +67,7 @@
     <t>Descricao</t>
   </si>
   <si>
-    <t>DesDataHoracricao</t>
+    <t>DataHora</t>
   </si>
   <si>
     <t>Caio Gonzaga</t>
@@ -102,7 +101,7 @@
 Teste.</t>
   </si>
   <si>
-    <t>3/17/2025 3:50 PM</t>
+    <t>18/03/2025 08:14</t>
   </si>
   <si>
     <t>Bruno Auzier</t>
@@ -120,11 +119,7 @@
     <t>Nozzle</t>
   </si>
   <si>
-    <t xml:space="preserve">Teste.
-Tese.</t>
-  </si>
-  <si>
-    <t>3/17/2025 3:51 PM</t>
+    <t>18/03/2025 08:16</t>
   </si>
   <si>
     <t>Maycon Nascimento</t>
@@ -154,13 +149,13 @@
     <t>Beta process</t>
   </si>
   <si>
-    <t>3/17/2025 3:53 PM</t>
+    <t>18/03/2025 08:17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="2">
     <font>
@@ -551,29 +546,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F50CB-CCF4-4A02-8BB3-6545B4B7DBF8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" bestFit="1" width="7.5703125" customWidth="1"/>
-    <col min="9" max="9" bestFit="1" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" bestFit="1" width="38.42578125" customWidth="1"/>
-    <col min="11" max="11" bestFit="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="6.125" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="5.75" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="8.375" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="12.875" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="13.75" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="7.75" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="7.625" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="16.875" customWidth="1"/>
+    <col min="10" max="10" bestFit="1" width="38.375" customWidth="1"/>
+    <col min="11" max="11" bestFit="1" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,45 +667,45 @@
         <v>26</v>
       </c>
       <c r="J3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -721,6 +716,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003A953F30D0EE8F469307B17CD3540C9C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ea79f87bf1a2afe83a39d29172c7935d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ec80d39e-601b-4802-9079-fb9d48824ad4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e1e20fa01357bb158138c1c7a7e7866d" ns3:_="">
     <xsd:import namespace="ec80d39e-601b-4802-9079-fb9d48824ad4"/>
@@ -908,22 +918,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C77CD2-0B03-49AB-9701-3BE6EE857365}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496DA2C0-4D13-441C-8312-EE1AAE92730E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ec80d39e-601b-4802-9079-fb9d48824ad4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99AC3F6A-E37A-4004-8E93-374F059EC1DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -939,28 +958,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C77CD2-0B03-49AB-9701-3BE6EE857365}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496DA2C0-4D13-441C-8312-EE1AAE92730E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ec80d39e-601b-4802-9079-fb9d48824ad4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update changes in BD.
</commit_message>
<xml_diff>
--- a/BancoDados.xlsx
+++ b/BancoDados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnscgonz\source\repos\caiogonz\HistoricoDefeitosProduto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mnsnt017\MNS-Files\Manufatura\Caio Gonzaga\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Funcionario</t>
   </si>
@@ -49,7 +49,7 @@
     <t>Setor</t>
   </si>
   <si>
-    <t>NumeroSerie</t>
+    <t>TrackID</t>
   </si>
   <si>
     <t>NomeProduto</t>
@@ -64,92 +64,52 @@
     <t>Suborigem</t>
   </si>
   <si>
-    <t>Descricao</t>
+    <t>Acao</t>
   </si>
   <si>
     <t>DataHora</t>
   </si>
   <si>
-    <t>Caio Gonzaga</t>
+    <t>Caio</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>FE01</t>
-  </si>
-  <si>
-    <t>FE FRESH</t>
-  </si>
-  <si>
-    <t>ZF5254T7ZL</t>
+    <t>FE09</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>JDKLSJ78JLK</t>
   </si>
   <si>
     <t>LAMU</t>
   </si>
   <si>
-    <t>Displaced weld deposition</t>
-  </si>
-  <si>
-    <t>Solder</t>
-  </si>
-  <si>
-    <t>Shifted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teste.
-Teste.</t>
-  </si>
-  <si>
-    <t>18/03/2025 08:14</t>
-  </si>
-  <si>
-    <t>Bruno Auzier</t>
-  </si>
-  <si>
-    <t>FE05</t>
-  </si>
-  <si>
-    <t>Lack of PM, obstructed, damaged, worn, life time, etc.</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Nozzle</t>
-  </si>
-  <si>
-    <t>18/03/2025 08:16</t>
-  </si>
-  <si>
-    <t>Maycon Nascimento</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>BE07</t>
-  </si>
-  <si>
-    <t>BE FRESH</t>
-  </si>
-  <si>
-    <t>ZF5254T7XJ</t>
-  </si>
-  <si>
-    <t>MANILA</t>
-  </si>
-  <si>
-    <t>Engineering activities (Process engineering, maintenance, testing, product, etc.)</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Beta process</t>
-  </si>
-  <si>
-    <t>18/03/2025 08:17</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>25/03/2025 11:22</t>
+  </si>
+  <si>
+    <t>Benda</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>JKDLS89JKL</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>TESTE</t>
+  </si>
+  <si>
+    <t>25/03/2025 11:24</t>
   </si>
 </sst>
 </file>
@@ -547,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -626,86 +586,51 @@
         <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -716,21 +641,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003A953F30D0EE8F469307B17CD3540C9C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ea79f87bf1a2afe83a39d29172c7935d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ec80d39e-601b-4802-9079-fb9d48824ad4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e1e20fa01357bb158138c1c7a7e7866d" ns3:_="">
     <xsd:import namespace="ec80d39e-601b-4802-9079-fb9d48824ad4"/>
@@ -918,31 +828,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C77CD2-0B03-49AB-9701-3BE6EE857365}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496DA2C0-4D13-441C-8312-EE1AAE92730E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ec80d39e-601b-4802-9079-fb9d48824ad4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99AC3F6A-E37A-4004-8E93-374F059EC1DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -958,4 +859,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C77CD2-0B03-49AB-9701-3BE6EE857365}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496DA2C0-4D13-441C-8312-EE1AAE92730E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ec80d39e-601b-4802-9079-fb9d48824ad4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>